<commit_message>
Fix CRS download, modularize
</commit_message>
<xml_diff>
--- a/output/current_sector_analysis.xlsx
+++ b/output/current_sector_analysis.xlsx
@@ -10,14 +10,14 @@
     <sheet name="sector_by_donor" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="sector_by_income" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="sector_by_recipient" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="sector_category_year" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="sector_year" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="sector_category_Year" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="sector_Year" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <si>
     <t xml:space="preserve">donor_type</t>
   </si>
@@ -37,31 +37,31 @@
     <t xml:space="preserve">Private</t>
   </si>
   <si>
-    <t xml:space="preserve">donor_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inter-American Development Bank [IDB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Bank for Reconstruction and Development [IBRD]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asian Development Bank [AsDB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Development Association [IDA]</t>
+    <t xml:space="preserve">DonorName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inter-American Development Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Bank for Reconstruction and Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asian Development Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Development Association</t>
   </si>
   <si>
     <t xml:space="preserve">Germany</t>
   </si>
   <si>
-    <t xml:space="preserve">European Bank for Reconstruction and Development [EBRD]</t>
+    <t xml:space="preserve">European Bank for Reconstruction and Development</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
   </si>
   <si>
-    <t xml:space="preserve">Asian Infrastructure Investment Bank [AIIB]</t>
+    <t xml:space="preserve">Asian Infrastructure Investment Bank</t>
   </si>
   <si>
     <t xml:space="preserve">EU Institutions</t>
@@ -73,27 +73,27 @@
     <t xml:space="preserve">Arab Fund (AFESD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Council of Europe Development Bank [CEB]</t>
+    <t xml:space="preserve">Council of Europe Development Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
   </si>
   <si>
     <t xml:space="preserve">Japan</t>
   </si>
   <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
     <t xml:space="preserve">United Arab Emirates</t>
   </si>
   <si>
-    <t xml:space="preserve">Central American Bank for Economic Integration [CABEI]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kuwait</t>
   </si>
   <si>
+    <t xml:space="preserve">Central American Bank for Economic Integration</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -106,10 +106,13 @@
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
+    <t xml:space="preserve">Private Infrastructure Development Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">Green Climate Fund [GCF]</t>
+    <t xml:space="preserve">Green Climate Fund</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar</t>
@@ -133,27 +136,30 @@
     <t xml:space="preserve">Ford Foundation</t>
   </si>
   <si>
+    <t xml:space="preserve">Howard G. Buffett Foundation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finland</t>
   </si>
   <si>
+    <t xml:space="preserve">African Development Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islamic Development Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEC Fund for International Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Environment Facility</t>
+  </si>
+  <si>
     <t xml:space="preserve">Norway</t>
   </si>
   <si>
-    <t xml:space="preserve">African Development Bank [AfDB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Islamic Development Bank [IsDB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEC Fund for International Development [OPEC Fund]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global Environment Facility [GEF]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belgium</t>
-  </si>
-  <si>
     <t xml:space="preserve">Luxembourg</t>
   </si>
   <si>
@@ -178,7 +184,7 @@
     <t xml:space="preserve">Australia</t>
   </si>
   <si>
-    <t xml:space="preserve">Climate Investment Funds [CIF]</t>
+    <t xml:space="preserve">Climate Investment Funds</t>
   </si>
   <si>
     <t xml:space="preserve">Conrad N. Hilton Foundation</t>
@@ -190,27 +196,27 @@
     <t xml:space="preserve">Ireland</t>
   </si>
   <si>
+    <t xml:space="preserve">Open Society Foundations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poland</t>
   </si>
   <si>
     <t xml:space="preserve">Citi Foundation</t>
   </si>
   <si>
-    <t xml:space="preserve">Open Society Foundations</t>
-  </si>
-  <si>
     <t xml:space="preserve">Austria</t>
   </si>
   <si>
     <t xml:space="preserve">Slovak Republic</t>
   </si>
   <si>
+    <t xml:space="preserve">Hungary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Van Leer Foundation</t>
   </si>
   <si>
-    <t xml:space="preserve">Hungary</t>
-  </si>
-  <si>
     <t xml:space="preserve">Czechia</t>
   </si>
   <si>
@@ -250,15 +256,15 @@
     <t xml:space="preserve">La Caixa Banking Foundation</t>
   </si>
   <si>
-    <t xml:space="preserve">income_group_code</t>
+    <t xml:space="preserve">IncomegroupName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMICs</t>
   </si>
   <si>
     <t xml:space="preserve">LMICs</t>
   </si>
   <si>
-    <t xml:space="preserve">UMICs</t>
-  </si>
-  <si>
     <t xml:space="preserve">LDCs</t>
   </si>
   <si>
@@ -271,18 +277,18 @@
     <t xml:space="preserve">Other LICs</t>
   </si>
   <si>
-    <t xml:space="preserve">recipient_name</t>
+    <t xml:space="preserve">RecipientName</t>
   </si>
   <si>
     <t xml:space="preserve">Mexico</t>
   </si>
   <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
     <t xml:space="preserve">Uzbekistan</t>
   </si>
   <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
     <t xml:space="preserve">Argentina</t>
   </si>
   <si>
@@ -304,12 +310,12 @@
     <t xml:space="preserve">Kenya</t>
   </si>
   <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ecuador</t>
   </si>
   <si>
-    <t xml:space="preserve">Ukraine</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pakistan</t>
   </si>
   <si>
@@ -328,19 +334,19 @@
     <t xml:space="preserve">Lebanon</t>
   </si>
   <si>
+    <t xml:space="preserve">Cabo Verde</t>
+  </si>
+  <si>
     <t xml:space="preserve">El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">Developing countries unspecified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cabo Verde</t>
+    <t xml:space="preserve">Bilateral, unspecified</t>
   </si>
   <si>
     <t xml:space="preserve">Bosnia and Herzegovina</t>
   </si>
   <si>
-    <t xml:space="preserve">Europe unspecified</t>
+    <t xml:space="preserve">Europe, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Jordan</t>
@@ -364,10 +370,10 @@
     <t xml:space="preserve">Mongolia</t>
   </si>
   <si>
-    <t xml:space="preserve">Palestinian Authority or West Bank and Gaza Strip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Africa unspecified</t>
+    <t xml:space="preserve">West Bank and Gaza Strip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Africa, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Bolivia</t>
@@ -376,24 +382,24 @@
     <t xml:space="preserve">South Africa</t>
   </si>
   <si>
+    <t xml:space="preserve">Georgia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rwanda</t>
   </si>
   <si>
-    <t xml:space="preserve">Georgia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uruguay</t>
   </si>
   <si>
+    <t xml:space="preserve">Yemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montenegro</t>
+  </si>
+  <si>
     <t xml:space="preserve">Myanmar</t>
   </si>
   <si>
-    <t xml:space="preserve">Yemen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montenegro</t>
-  </si>
-  <si>
     <t xml:space="preserve">North Macedonia</t>
   </si>
   <si>
@@ -415,22 +421,22 @@
     <t xml:space="preserve">Bhutan</t>
   </si>
   <si>
-    <t xml:space="preserve">Africa unspecified</t>
+    <t xml:space="preserve">Africa, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Honduras</t>
   </si>
   <si>
     <t xml:space="preserve">Nepal</t>
   </si>
   <si>
-    <t xml:space="preserve">Honduras</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mozambique</t>
   </si>
   <si>
     <t xml:space="preserve">Sudan</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub-Saharan Africa unspecified</t>
+    <t xml:space="preserve">South of Sahara, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Moldova</t>
@@ -442,31 +448,34 @@
     <t xml:space="preserve">Uganda</t>
   </si>
   <si>
-    <t xml:space="preserve">China (People’s Republic of)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Armenia</t>
   </si>
   <si>
+    <t xml:space="preserve">China (People's Republic of)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kyrgyzstan</t>
   </si>
   <si>
+    <t xml:space="preserve">North of Sahara, regional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ghana</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Africa unspecified</t>
+    <t xml:space="preserve">Mali</t>
   </si>
   <si>
     <t xml:space="preserve">Suriname</t>
   </si>
   <si>
-    <t xml:space="preserve">Mali</t>
+    <t xml:space="preserve">Syrian Arab Republic</t>
   </si>
   <si>
     <t xml:space="preserve">Dominica</t>
   </si>
   <si>
-    <t xml:space="preserve">Syrian Arab Republic</t>
+    <t xml:space="preserve">Democratic Republic of the Congo</t>
   </si>
   <si>
     <t xml:space="preserve">Tanzania</t>
@@ -475,9 +484,6 @@
     <t xml:space="preserve">Fiji</t>
   </si>
   <si>
-    <t xml:space="preserve">Democratic Republic of the Congo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dominican Republic</t>
   </si>
   <si>
@@ -490,7 +496,7 @@
     <t xml:space="preserve">Kiribati</t>
   </si>
   <si>
-    <t xml:space="preserve">Asia unspecified</t>
+    <t xml:space="preserve">Asia, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Guatemala</t>
@@ -505,7 +511,7 @@
     <t xml:space="preserve">Cambodia</t>
   </si>
   <si>
-    <t xml:space="preserve">Central America and the Caribbean unspecified</t>
+    <t xml:space="preserve">Caribbean &amp; Central America, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Tonga</t>
@@ -514,12 +520,12 @@
     <t xml:space="preserve">Malaysia</t>
   </si>
   <si>
+    <t xml:space="preserve">America, regional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albania</t>
   </si>
   <si>
-    <t xml:space="preserve">America unspecified</t>
-  </si>
-  <si>
     <t xml:space="preserve">Seychelles</t>
   </si>
   <si>
@@ -529,7 +535,7 @@
     <t xml:space="preserve">Cameroon</t>
   </si>
   <si>
-    <t xml:space="preserve">South America unspecified</t>
+    <t xml:space="preserve">South America, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Burkina Faso</t>
@@ -541,16 +547,19 @@
     <t xml:space="preserve">Zambia</t>
   </si>
   <si>
-    <t xml:space="preserve">Central Asia unspecified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Côte d’Ivoire</t>
+    <t xml:space="preserve">Central Asia, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burundi</t>
   </si>
   <si>
     <t xml:space="preserve">Madagascar</t>
   </si>
   <si>
-    <t xml:space="preserve">Burundi</t>
+    <t xml:space="preserve">Cuba</t>
   </si>
   <si>
     <t xml:space="preserve">Somalia</t>
@@ -559,28 +568,28 @@
     <t xml:space="preserve">Samoa</t>
   </si>
   <si>
-    <t xml:space="preserve">Cuba</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comoros</t>
   </si>
   <si>
+    <t xml:space="preserve">Malawi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zimbabwe</t>
   </si>
   <si>
-    <t xml:space="preserve">Liberia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malawi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central America unspecified</t>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central America, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">Southern Africa unspecified</t>
+    <t xml:space="preserve">Southern Africa, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Niger</t>
@@ -592,15 +601,12 @@
     <t xml:space="preserve">Chad</t>
   </si>
   <si>
-    <t xml:space="preserve">Nigeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lao People’s Democratic Republic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vanuatu</t>
   </si>
   <si>
+    <t xml:space="preserve">Lao People's Democratic Republic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Angola</t>
   </si>
   <si>
@@ -625,12 +631,12 @@
     <t xml:space="preserve">Iran</t>
   </si>
   <si>
+    <t xml:space="preserve">Azerbaijan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Benin</t>
   </si>
   <si>
-    <t xml:space="preserve">Azerbaijan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mauritania</t>
   </si>
   <si>
@@ -646,10 +652,10 @@
     <t xml:space="preserve">Kosovo</t>
   </si>
   <si>
-    <t xml:space="preserve">Far East Asia unspecified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Asia unspecified</t>
+    <t xml:space="preserve">Far East Asia, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Asia, regional</t>
   </si>
   <si>
     <t xml:space="preserve">Tuvalu</t>
@@ -670,16 +676,16 @@
     <t xml:space="preserve">Mauritius</t>
   </si>
   <si>
-    <t xml:space="preserve">States ex-Yugoslavia unspecified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Democratic People’s Republic of Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle East unspecified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
+    <t xml:space="preserve">States Ex-Yugoslavia unspecified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic People's Republic of Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle East, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
   </si>
   <si>
     <t xml:space="preserve">ODA</t>
@@ -1246,7 +1252,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>9714.62115600002</v>
+        <v>10239.21746</v>
       </c>
     </row>
     <row r="3">
@@ -1254,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1708.535457</v>
+        <v>1830.96223500001</v>
       </c>
     </row>
     <row r="4">
@@ -1262,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>452.73471</v>
+        <v>476.100212</v>
       </c>
     </row>
     <row r="5">
@@ -1270,7 +1276,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>29.824956</v>
+        <v>41.562424</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>3701.463644</v>
+        <v>3882.337477</v>
       </c>
     </row>
     <row r="3">
@@ -1309,7 +1315,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>2235.443376</v>
+        <v>2344.739283</v>
       </c>
     </row>
     <row r="4">
@@ -1317,7 +1323,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>1494.63312</v>
+        <v>1567.061369</v>
       </c>
     </row>
     <row r="5">
@@ -1325,7 +1331,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>662.741417</v>
+        <v>695.001</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1339,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>630.93975</v>
+        <v>690.385126999999</v>
       </c>
     </row>
     <row r="7">
@@ -1341,7 +1347,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>609.169884</v>
+        <v>638.918353</v>
       </c>
     </row>
     <row r="8">
@@ -1349,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>439.156556</v>
+        <v>476.40375</v>
       </c>
     </row>
     <row r="9">
@@ -1357,7 +1363,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>284.408678</v>
+        <v>298.368512</v>
       </c>
     </row>
     <row r="10">
@@ -1365,7 +1371,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>254.63142</v>
+        <v>278.221393</v>
       </c>
     </row>
     <row r="11">
@@ -1373,7 +1379,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>228.198982</v>
+        <v>239.667382</v>
       </c>
     </row>
     <row r="12">
@@ -1381,7 +1387,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>157.520635</v>
+        <v>167.438419</v>
       </c>
     </row>
     <row r="13">
@@ -1389,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>151.580294</v>
+        <v>159.062058</v>
       </c>
     </row>
     <row r="14">
@@ -1397,7 +1403,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>116.469624</v>
+        <v>125.176022</v>
       </c>
     </row>
     <row r="15">
@@ -1405,7 +1411,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>115.514327</v>
+        <v>123.103349</v>
       </c>
     </row>
     <row r="16">
@@ -1413,7 +1419,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>111.174619</v>
+        <v>113.25017</v>
       </c>
     </row>
     <row r="17">
@@ -1421,7 +1427,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>101.162009</v>
+        <v>106.038893</v>
       </c>
     </row>
     <row r="18">
@@ -1429,7 +1435,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>96.184906</v>
+        <v>100.841407</v>
       </c>
     </row>
     <row r="19">
@@ -1437,7 +1443,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>96.065075</v>
+        <v>100.584263</v>
       </c>
     </row>
     <row r="20">
@@ -1445,7 +1451,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>53.172467</v>
+        <v>55.173378</v>
       </c>
     </row>
     <row r="21">
@@ -1453,7 +1459,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>45.659157</v>
+        <v>44.808794</v>
       </c>
     </row>
     <row r="22">
@@ -1461,7 +1467,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>42.460749</v>
+        <v>42.884766</v>
       </c>
     </row>
     <row r="23">
@@ -1469,7 +1475,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>38.348322</v>
+        <v>38.7606249999999</v>
       </c>
     </row>
     <row r="24">
@@ -1477,7 +1483,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>24.348191</v>
+        <v>37.361541</v>
       </c>
     </row>
     <row r="25">
@@ -1485,7 +1491,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>20.555179</v>
+        <v>26.237135</v>
       </c>
     </row>
     <row r="26">
@@ -1493,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>18.502781</v>
+        <v>21.583</v>
       </c>
     </row>
     <row r="27">
@@ -1501,7 +1507,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>14.681441</v>
+        <v>19.407022</v>
       </c>
     </row>
     <row r="28">
@@ -1509,7 +1515,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>14.22759</v>
+        <v>16.055492</v>
       </c>
     </row>
     <row r="29">
@@ -1517,7 +1523,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="n">
-        <v>13.20938</v>
+        <v>15.580147</v>
       </c>
     </row>
     <row r="30">
@@ -1525,7 +1531,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="n">
-        <v>12.623959</v>
+        <v>13.513427</v>
       </c>
     </row>
     <row r="31">
@@ -1533,7 +1539,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="n">
-        <v>12.338702</v>
+        <v>13.258792</v>
       </c>
     </row>
     <row r="32">
@@ -1541,7 +1547,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>9.916816</v>
+        <v>12.287527</v>
       </c>
     </row>
     <row r="33">
@@ -1549,7 +1555,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="n">
-        <v>9.423672</v>
+        <v>10.279241</v>
       </c>
     </row>
     <row r="34">
@@ -1557,7 +1563,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>9.226359</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="35">
@@ -1565,7 +1571,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="n">
-        <v>8.668864</v>
+        <v>10.091007</v>
       </c>
     </row>
     <row r="36">
@@ -1573,7 +1579,7 @@
         <v>41</v>
       </c>
       <c r="B36" t="n">
-        <v>7.871286</v>
+        <v>9.104804</v>
       </c>
     </row>
     <row r="37">
@@ -1581,7 +1587,7 @@
         <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>7.790524</v>
+        <v>8.236642</v>
       </c>
     </row>
     <row r="38">
@@ -1589,7 +1595,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>7.410194</v>
+        <v>8.15598</v>
       </c>
     </row>
     <row r="39">
@@ -1597,7 +1603,7 @@
         <v>44</v>
       </c>
       <c r="B39" t="n">
-        <v>7.328791</v>
+        <v>7.935646</v>
       </c>
     </row>
     <row r="40">
@@ -1605,7 +1611,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>6.32606</v>
+        <v>7.768332</v>
       </c>
     </row>
     <row r="41">
@@ -1613,7 +1619,7 @@
         <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>5.530054</v>
+        <v>7.6788</v>
       </c>
     </row>
     <row r="42">
@@ -1621,7 +1627,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="n">
-        <v>5.078191</v>
+        <v>6.793007</v>
       </c>
     </row>
     <row r="43">
@@ -1629,7 +1635,7 @@
         <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>4.980933</v>
+        <v>6.465903</v>
       </c>
     </row>
     <row r="44">
@@ -1637,7 +1643,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="n">
-        <v>4.905669</v>
+        <v>5.513149</v>
       </c>
     </row>
     <row r="45">
@@ -1645,7 +1651,7 @@
         <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>3.005065</v>
+        <v>5.163372</v>
       </c>
     </row>
     <row r="46">
@@ -1653,7 +1659,7 @@
         <v>51</v>
       </c>
       <c r="B46" t="n">
-        <v>2.345671</v>
+        <v>4.954058</v>
       </c>
     </row>
     <row r="47">
@@ -1661,7 +1667,7 @@
         <v>52</v>
       </c>
       <c r="B47" t="n">
-        <v>1.96441</v>
+        <v>3.384646</v>
       </c>
     </row>
     <row r="48">
@@ -1669,7 +1675,7 @@
         <v>53</v>
       </c>
       <c r="B48" t="n">
-        <v>0.970497</v>
+        <v>2.60938</v>
       </c>
     </row>
     <row r="49">
@@ -1677,7 +1683,7 @@
         <v>54</v>
       </c>
       <c r="B49" t="n">
-        <v>0.906691</v>
+        <v>1.962716</v>
       </c>
     </row>
     <row r="50">
@@ -1685,7 +1691,7 @@
         <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>0.860672</v>
+        <v>1.017598</v>
       </c>
     </row>
     <row r="51">
@@ -1693,7 +1699,7 @@
         <v>56</v>
       </c>
       <c r="B51" t="n">
-        <v>0.693874</v>
+        <v>0.939742</v>
       </c>
     </row>
     <row r="52">
@@ -1701,7 +1707,7 @@
         <v>57</v>
       </c>
       <c r="B52" t="n">
-        <v>0.462468</v>
+        <v>0.901795</v>
       </c>
     </row>
     <row r="53">
@@ -1709,7 +1715,7 @@
         <v>58</v>
       </c>
       <c r="B53" t="n">
-        <v>0.450751</v>
+        <v>0.74481</v>
       </c>
     </row>
     <row r="54">
@@ -1717,7 +1723,7 @@
         <v>59</v>
       </c>
       <c r="B54" t="n">
-        <v>0.428504</v>
+        <v>0.667673</v>
       </c>
     </row>
     <row r="55">
@@ -1725,7 +1731,7 @@
         <v>60</v>
       </c>
       <c r="B55" t="n">
-        <v>0.422677</v>
+        <v>0.538647</v>
       </c>
     </row>
     <row r="56">
@@ -1733,7 +1739,7 @@
         <v>61</v>
       </c>
       <c r="B56" t="n">
-        <v>0.343844</v>
+        <v>0.467292</v>
       </c>
     </row>
     <row r="57">
@@ -1741,7 +1747,7 @@
         <v>62</v>
       </c>
       <c r="B57" t="n">
-        <v>0.260116</v>
+        <v>0.459085</v>
       </c>
     </row>
     <row r="58">
@@ -1749,7 +1755,7 @@
         <v>63</v>
       </c>
       <c r="B58" t="n">
-        <v>0.25355</v>
+        <v>0.389035</v>
       </c>
     </row>
     <row r="59">
@@ -1757,7 +1763,7 @@
         <v>64</v>
       </c>
       <c r="B59" t="n">
-        <v>0.226156</v>
+        <v>0.305639</v>
       </c>
     </row>
     <row r="60">
@@ -1765,7 +1771,7 @@
         <v>65</v>
       </c>
       <c r="B60" t="n">
-        <v>0.20949</v>
+        <v>0.289735</v>
       </c>
     </row>
     <row r="61">
@@ -1773,7 +1779,7 @@
         <v>66</v>
       </c>
       <c r="B61" t="n">
-        <v>0.137491</v>
+        <v>0.261873</v>
       </c>
     </row>
     <row r="62">
@@ -1781,7 +1787,7 @@
         <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>0.130786</v>
+        <v>0.21956</v>
       </c>
     </row>
     <row r="63">
@@ -1789,7 +1795,7 @@
         <v>68</v>
       </c>
       <c r="B63" t="n">
-        <v>0.118868</v>
+        <v>0.149296</v>
       </c>
     </row>
     <row r="64">
@@ -1797,7 +1803,7 @@
         <v>69</v>
       </c>
       <c r="B64" t="n">
-        <v>0.105153</v>
+        <v>0.135552</v>
       </c>
     </row>
     <row r="65">
@@ -1805,7 +1811,7 @@
         <v>70</v>
       </c>
       <c r="B65" t="n">
-        <v>0.092607</v>
+        <v>0.116933</v>
       </c>
     </row>
     <row r="66">
@@ -1813,7 +1819,7 @@
         <v>71</v>
       </c>
       <c r="B66" t="n">
-        <v>0.082989</v>
+        <v>0.11272</v>
       </c>
     </row>
     <row r="67">
@@ -1821,7 +1827,7 @@
         <v>72</v>
       </c>
       <c r="B67" t="n">
-        <v>0.061254</v>
+        <v>0.096849</v>
       </c>
     </row>
     <row r="68">
@@ -1829,7 +1835,7 @@
         <v>73</v>
       </c>
       <c r="B68" t="n">
-        <v>0.048183</v>
+        <v>0.093428</v>
       </c>
     </row>
     <row r="69">
@@ -1837,7 +1843,7 @@
         <v>74</v>
       </c>
       <c r="B69" t="n">
-        <v>0.042828</v>
+        <v>0.075399</v>
       </c>
     </row>
     <row r="70">
@@ -1845,7 +1851,7 @@
         <v>75</v>
       </c>
       <c r="B70" t="n">
-        <v>0.031549</v>
+        <v>0.054488</v>
       </c>
     </row>
     <row r="71">
@@ -1853,7 +1859,23 @@
         <v>76</v>
       </c>
       <c r="B71" t="n">
-        <v>0.016488</v>
+        <v>0.046191</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.034345</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.01809</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1895,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1881,50 +1903,50 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" t="n">
-        <v>5614.461843</v>
+        <v>6289.843983</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B3" t="n">
-        <v>5294.95456</v>
+        <v>5273.008783</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" t="n">
-        <v>590.959026</v>
+        <v>593.644478</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5" t="n">
-        <v>341.523139</v>
+        <v>364.136825</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" t="n">
-        <v>55.928279</v>
+        <v>58.63966</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="n">
-        <v>7.889432</v>
+        <v>8.568602</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +1966,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1952,1090 +1974,1090 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
-        <v>1465.551417</v>
+        <v>1539.871921</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" t="n">
-        <v>1134.913901</v>
+        <v>1194.221028</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" t="n">
-        <v>1108.583257</v>
+        <v>1190.041532</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B5" t="n">
-        <v>1075.195517</v>
+        <v>1127.17959</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
-        <v>982.243278</v>
+        <v>1030.917093</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
-        <v>713.884797</v>
+        <v>749.163294</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
-        <v>642.729372</v>
+        <v>674.348322</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9" t="n">
-        <v>418.199534</v>
+        <v>436.263702</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B10" t="n">
-        <v>364.11573</v>
+        <v>391.239633</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B11" t="n">
-        <v>322.101878</v>
+        <v>355.192146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B12" t="n">
-        <v>212.215273</v>
+        <v>236.47923</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B13" t="n">
-        <v>211.507839</v>
+        <v>224.693465</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B14" t="n">
-        <v>202.186931</v>
+        <v>212.092362</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B15" t="n">
-        <v>155.888539</v>
+        <v>164.212476</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B16" t="n">
-        <v>153.312063</v>
+        <v>164.194039</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B17" t="n">
-        <v>149.986749</v>
+        <v>157.391489</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18" t="n">
-        <v>129.577222</v>
+        <v>137.890461</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B19" t="n">
-        <v>124.160679</v>
+        <v>130.478304</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B20" t="n">
-        <v>115.812968</v>
+        <v>123.28804</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B21" t="n">
-        <v>113.021382</v>
+        <v>121.427888</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B22" t="n">
-        <v>111.347533</v>
+        <v>120.065569</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B23" t="n">
-        <v>100.922846</v>
+        <v>106.50452</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B24" t="n">
-        <v>98.106736</v>
+        <v>106.251507</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B25" t="n">
-        <v>91.368638</v>
+        <v>95.993436</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B26" t="n">
-        <v>90.622464</v>
+        <v>95.681702</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B27" t="n">
-        <v>87.89065</v>
+        <v>92.011249</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B28" t="n">
-        <v>85.061879</v>
+        <v>89.011746</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B29" t="n">
-        <v>83.199899</v>
+        <v>88.411864</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B30" t="n">
-        <v>75.838976</v>
+        <v>79.424102</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B31" t="n">
-        <v>71.396831</v>
+        <v>73.544646</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B32" t="n">
-        <v>69.457378</v>
+        <v>73.124516</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B33" t="n">
-        <v>64.395072</v>
+        <v>67.547231</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B34" t="n">
-        <v>60.447953</v>
+        <v>63.388151</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B35" t="n">
-        <v>57.733125</v>
+        <v>62.575659</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B36" t="n">
-        <v>57.434602</v>
+        <v>60.325484</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B37" t="n">
-        <v>57.022546</v>
+        <v>60.074368</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B38" t="n">
-        <v>53.00352</v>
+        <v>55.562461</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B39" t="n">
-        <v>51.230961</v>
+        <v>53.756212</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B40" t="n">
-        <v>43.365888</v>
+        <v>44.446692</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B41" t="n">
-        <v>42.367468</v>
+        <v>43.159959</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B42" t="n">
-        <v>41.035015</v>
+        <v>42.481656</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B43" t="n">
-        <v>39.826824</v>
+        <v>41.803735</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B44" t="n">
-        <v>38.201167</v>
+        <v>41.070323</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B45" t="n">
-        <v>37.945597</v>
+        <v>39.477218</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B46" t="n">
-        <v>36.472442</v>
+        <v>38.123079</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B47" t="n">
-        <v>32.535001</v>
+        <v>36.184278</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B48" t="n">
-        <v>31.737368</v>
+        <v>34.719334</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B49" t="n">
-        <v>24.124964</v>
+        <v>25.053723</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B50" t="n">
-        <v>21.689463</v>
+        <v>22.974542</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B51" t="n">
-        <v>20.765627</v>
+        <v>21.317807</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B52" t="n">
-        <v>20.347247</v>
+        <v>21.074975</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B53" t="n">
-        <v>19.095225</v>
+        <v>19.92917</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B54" t="n">
-        <v>16.826933</v>
+        <v>17.658225</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" t="n">
-        <v>16.573479</v>
+        <v>17.457252</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B56" t="n">
-        <v>15.988328</v>
+        <v>16.777437</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B57" t="n">
-        <v>15.092637</v>
+        <v>15.829109</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B58" t="n">
-        <v>14.611138</v>
+        <v>15.665564</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B59" t="n">
-        <v>14.108474</v>
+        <v>15.121938</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B60" t="n">
-        <v>13.923985</v>
+        <v>14.782812</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B61" t="n">
-        <v>11.868535</v>
+        <v>12.488421</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B62" t="n">
-        <v>10.919306</v>
+        <v>11.893752</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B63" t="n">
-        <v>10.846415</v>
+        <v>11.781719</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B64" t="n">
-        <v>8.972202</v>
+        <v>9.448286</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B65" t="n">
-        <v>8.951129</v>
+        <v>9.38833</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B66" t="n">
-        <v>8.029161</v>
+        <v>8.563024</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B67" t="n">
-        <v>7.884259</v>
+        <v>8.419594</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B68" t="n">
-        <v>7.297509</v>
+        <v>7.715791</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B69" t="n">
-        <v>7.236837</v>
+        <v>7.539031</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B70" t="n">
-        <v>7.186099</v>
+        <v>7.44704</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B71" t="n">
-        <v>6.367343</v>
+        <v>6.682171</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B72" t="n">
-        <v>6.101454</v>
+        <v>6.471171</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B73" t="n">
-        <v>5.948505</v>
+        <v>6.237327</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B74" t="n">
-        <v>5.524039</v>
+        <v>5.650731</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B75" t="n">
-        <v>5.445497</v>
+        <v>5.638737</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B76" t="n">
-        <v>5.155401</v>
+        <v>5.612666</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B77" t="n">
-        <v>3.984471</v>
+        <v>4.164593</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B78" t="n">
-        <v>3.65633</v>
+        <v>3.874099</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B79" t="n">
-        <v>3.372977</v>
+        <v>3.66439</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B80" t="n">
-        <v>3.300314</v>
+        <v>3.451578</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B81" t="n">
-        <v>3.105564</v>
+        <v>3.255531</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B82" t="n">
-        <v>3.055237</v>
+        <v>3.201648</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B83" t="n">
-        <v>2.986917</v>
+        <v>3.177172</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B84" t="n">
-        <v>2.832543</v>
+        <v>3.124104</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B85" t="n">
-        <v>2.514855</v>
+        <v>2.641744</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B86" t="n">
-        <v>2.479305</v>
+        <v>2.592978</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B87" t="n">
-        <v>2.305742</v>
+        <v>2.516507</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B88" t="n">
-        <v>2.274084</v>
+        <v>2.440971</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B89" t="n">
-        <v>2.12812</v>
+        <v>2.284619</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B90" t="n">
-        <v>1.972642</v>
+        <v>2.071842</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B91" t="n">
-        <v>1.971916</v>
+        <v>2.048599</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B92" t="n">
-        <v>1.561248</v>
+        <v>1.696388</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B93" t="n">
-        <v>1.345136</v>
+        <v>1.396945</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B94" t="n">
-        <v>1.289657</v>
+        <v>1.377437</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B95" t="n">
-        <v>1.282522</v>
+        <v>1.364556</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B96" t="n">
-        <v>1.176227</v>
+        <v>1.232603</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B97" t="n">
-        <v>1.147537</v>
+        <v>1.189207</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B98" t="n">
-        <v>1.134325</v>
+        <v>1.173632</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B99" t="n">
-        <v>1.072285</v>
+        <v>1.122665</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B100" t="n">
-        <v>1.04887</v>
+        <v>1.102966</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B101" t="n">
-        <v>0.960584</v>
+        <v>1.043161</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B102" t="n">
-        <v>0.86721</v>
+        <v>1.042371</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B103" t="n">
-        <v>0.802861</v>
+        <v>0.942748</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B104" t="n">
-        <v>0.740576</v>
+        <v>0.811675</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B105" t="n">
-        <v>0.599364</v>
+        <v>0.772413</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B106" t="n">
-        <v>0.587628</v>
+        <v>0.648789</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B107" t="n">
-        <v>0.578915</v>
+        <v>0.633972</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B108" t="n">
-        <v>0.546678</v>
+        <v>0.626507</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B109" t="n">
-        <v>0.529433</v>
+        <v>0.598894</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B110" t="n">
-        <v>0.495469</v>
+        <v>0.509613</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B111" t="n">
-        <v>0.489149</v>
+        <v>0.482309</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B112" t="n">
-        <v>0.466428</v>
+        <v>0.477547</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B113" t="n">
-        <v>0.409904</v>
+        <v>0.435455</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B114" t="n">
-        <v>0.401343</v>
+        <v>0.407135</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B115" t="n">
-        <v>0.369072</v>
+        <v>0.401205</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B116" t="n">
-        <v>0.305359</v>
+        <v>0.325003</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B117" t="n">
-        <v>0.296228</v>
+        <v>0.291993</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B118" t="n">
-        <v>0.199474</v>
+        <v>0.204966</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B119" t="n">
-        <v>0.172873</v>
+        <v>0.175638</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B120" t="n">
-        <v>0.152089</v>
+        <v>0.159551</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B121" t="n">
-        <v>0.146046</v>
+        <v>0.158557</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B122" t="n">
-        <v>0.134849</v>
+        <v>0.147962</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B123" t="n">
-        <v>0.108489</v>
+        <v>0.113934</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B124" t="n">
-        <v>0.080482</v>
+        <v>0.086556</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B125" t="n">
-        <v>0.041754</v>
+        <v>0.044215</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B126" t="n">
-        <v>0.040532</v>
+        <v>0.042802</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B127" t="n">
-        <v>0.034537</v>
+        <v>0.037249</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B128" t="n">
-        <v>0.033028</v>
+        <v>0.035865</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B129" t="n">
-        <v>0.014839</v>
+        <v>0.014429</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B130" t="n">
-        <v>0.014149</v>
+        <v>0.014418</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B131" t="n">
-        <v>0.01353</v>
+        <v>0.013157</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B132" t="n">
-        <v>0.012956</v>
+        <v>0.012857</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B133" t="n">
-        <v>0.012371</v>
+        <v>0.012606</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B134" t="n">
-        <v>0.009071</v>
+        <v>0.008822</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B135" t="n">
-        <v>0.007006</v>
+        <v>0.008437</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B136" t="n">
-        <v>0.005173</v>
+        <v>0.005578</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B137" t="n">
-        <v>0.00011</v>
+        <v>0.000111</v>
       </c>
     </row>
   </sheetData>
@@ -3055,13 +3077,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -3072,13 +3094,13 @@
         <v>2014</v>
       </c>
       <c r="B2" t="n">
-        <v>265.819998</v>
+        <v>283.236531</v>
       </c>
       <c r="C2" t="n">
-        <v>621.503808</v>
+        <v>649.977044</v>
       </c>
       <c r="D2" t="n">
-        <v>0.712874</v>
+        <v>0.743859</v>
       </c>
     </row>
     <row r="3">
@@ -3086,13 +3108,13 @@
         <v>2015</v>
       </c>
       <c r="B3" t="n">
-        <v>310.073139</v>
+        <v>331.182781</v>
       </c>
       <c r="C3" t="n">
-        <v>749.409626</v>
+        <v>784.389708</v>
       </c>
       <c r="D3" t="n">
-        <v>0.772996</v>
+        <v>0.839404</v>
       </c>
     </row>
     <row r="4">
@@ -3100,13 +3122,13 @@
         <v>2016</v>
       </c>
       <c r="B4" t="n">
-        <v>350.07006</v>
+        <v>370.930406</v>
       </c>
       <c r="C4" t="n">
-        <v>480.405993</v>
+        <v>504.645266</v>
       </c>
       <c r="D4" t="n">
-        <v>2.041958</v>
+        <v>2.146965</v>
       </c>
     </row>
     <row r="5">
@@ -3114,13 +3136,13 @@
         <v>2017</v>
       </c>
       <c r="B5" t="n">
-        <v>581.985478</v>
+        <v>626.300829999999</v>
       </c>
       <c r="C5" t="n">
-        <v>624.933067</v>
+        <v>656.3597</v>
       </c>
       <c r="D5" t="n">
-        <v>7.749542</v>
+        <v>8.174658</v>
       </c>
     </row>
     <row r="6">
@@ -3128,13 +3150,13 @@
         <v>2018</v>
       </c>
       <c r="B6" t="n">
-        <v>372.008704</v>
+        <v>396.210794</v>
       </c>
       <c r="C6" t="n">
-        <v>519.807648</v>
+        <v>546.319853</v>
       </c>
       <c r="D6" t="n">
-        <v>4.441862</v>
+        <v>4.631842</v>
       </c>
     </row>
     <row r="7">
@@ -3142,13 +3164,13 @@
         <v>2019</v>
       </c>
       <c r="B7" t="n">
-        <v>557.043863</v>
+        <v>590.063265</v>
       </c>
       <c r="C7" t="n">
-        <v>1444.084605</v>
+        <v>1518.178</v>
       </c>
       <c r="D7" t="n">
-        <v>7.268529</v>
+        <v>7.577422</v>
       </c>
     </row>
     <row r="8">
@@ -3156,13 +3178,13 @@
         <v>2020</v>
       </c>
       <c r="B8" t="n">
-        <v>451.49774</v>
+        <v>473.850568</v>
       </c>
       <c r="C8" t="n">
-        <v>1708.340234</v>
+        <v>1792.50534</v>
       </c>
       <c r="D8" t="n">
-        <v>3.412551</v>
+        <v>3.549975</v>
       </c>
     </row>
     <row r="9">
@@ -3170,13 +3192,13 @@
         <v>2021</v>
       </c>
       <c r="B9" t="n">
-        <v>178.70199</v>
+        <v>193.373539</v>
       </c>
       <c r="C9" t="n">
-        <v>698.930706</v>
+        <v>763.144768</v>
       </c>
       <c r="D9" t="n">
-        <v>2.557163</v>
+        <v>2.689734</v>
       </c>
     </row>
     <row r="10">
@@ -3184,13 +3206,13 @@
         <v>2022</v>
       </c>
       <c r="B10" t="n">
-        <v>229.535336</v>
+        <v>244.504761</v>
       </c>
       <c r="C10" t="n">
-        <v>962.571676</v>
+        <v>1015.903745</v>
       </c>
       <c r="D10" t="n">
-        <v>0.867481</v>
+        <v>1.108565</v>
       </c>
     </row>
     <row r="11">
@@ -3198,13 +3220,13 @@
         <v>2023</v>
       </c>
       <c r="B11" t="n">
-        <v>184.803379</v>
+        <v>194.389197</v>
       </c>
       <c r="C11" t="n">
-        <v>509.648243</v>
+        <v>532.186989</v>
       </c>
       <c r="D11" t="n">
-        <v>74.71603</v>
+        <v>88.726822</v>
       </c>
     </row>
   </sheetData>
@@ -3224,13 +3246,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -3238,10 +3260,10 @@
         <v>2014</v>
       </c>
       <c r="B2" t="n">
-        <v>220.590817</v>
+        <v>230.576004</v>
       </c>
       <c r="C2" t="n">
-        <v>667.445863</v>
+        <v>703.38143</v>
       </c>
     </row>
     <row r="3">
@@ -3249,10 +3271,10 @@
         <v>2015</v>
       </c>
       <c r="B3" t="n">
-        <v>569.004285</v>
+        <v>598.0885</v>
       </c>
       <c r="C3" t="n">
-        <v>491.251476</v>
+        <v>518.323393</v>
       </c>
     </row>
     <row r="4">
@@ -3260,10 +3282,10 @@
         <v>2016</v>
       </c>
       <c r="B4" t="n">
-        <v>337.430898</v>
+        <v>354.863361</v>
       </c>
       <c r="C4" t="n">
-        <v>495.087113</v>
+        <v>522.859276</v>
       </c>
     </row>
     <row r="5">
@@ -3271,10 +3293,10 @@
         <v>2017</v>
       </c>
       <c r="B5" t="n">
-        <v>464.40998</v>
+        <v>488.668093</v>
       </c>
       <c r="C5" t="n">
-        <v>750.258107</v>
+        <v>802.167095</v>
       </c>
     </row>
     <row r="6">
@@ -3282,10 +3304,10 @@
         <v>2018</v>
       </c>
       <c r="B6" t="n">
-        <v>560.372002</v>
+        <v>591.872359</v>
       </c>
       <c r="C6" t="n">
-        <v>335.886212</v>
+        <v>355.29013</v>
       </c>
     </row>
     <row r="7">
@@ -3293,10 +3315,10 @@
         <v>2019</v>
       </c>
       <c r="B7" t="n">
-        <v>1460.276904</v>
+        <v>1537.080369</v>
       </c>
       <c r="C7" t="n">
-        <v>548.120093</v>
+        <v>578.738318</v>
       </c>
     </row>
     <row r="8">
@@ -3304,10 +3326,10 @@
         <v>2020</v>
       </c>
       <c r="B8" t="n">
-        <v>1681.50942</v>
+        <v>1766.954544</v>
       </c>
       <c r="C8" t="n">
-        <v>481.741105</v>
+        <v>502.951339</v>
       </c>
     </row>
     <row r="9">
@@ -3315,10 +3337,10 @@
         <v>2021</v>
       </c>
       <c r="B9" t="n">
-        <v>523.584168</v>
+        <v>581.574094</v>
       </c>
       <c r="C9" t="n">
-        <v>356.605691</v>
+        <v>377.633947</v>
       </c>
     </row>
     <row r="10">
@@ -3326,10 +3348,10 @@
         <v>2022</v>
       </c>
       <c r="B10" t="n">
-        <v>690.545155</v>
+        <v>730.315401000001</v>
       </c>
       <c r="C10" t="n">
-        <v>502.429338</v>
+        <v>531.20167</v>
       </c>
     </row>
     <row r="11">
@@ -3337,10 +3359,10 @@
         <v>2023</v>
       </c>
       <c r="B11" t="n">
-        <v>449.375777</v>
+        <v>481.469684</v>
       </c>
       <c r="C11" t="n">
-        <v>319.791875</v>
+        <v>333.833324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>